<commit_message>
AWRSS Sprint 1 and Soccer pred challenge
</commit_message>
<xml_diff>
--- a/Writing/22-23/23_01_001.xlsx
+++ b/Writing/22-23/23_01_001.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yashkarle/soccer-ds-stats/Writing/22-23/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC9D514-D88D-254E-900B-F967E8E84071}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F9226B-9560-DB4E-9D1E-9448EED0E7D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19080" activeTab="2" xr2:uid="{E93522CD-A16F-944B-B80D-1F57AE0445AA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19080" activeTab="6" xr2:uid="{E93522CD-A16F-944B-B80D-1F57AE0445AA}"/>
   </bookViews>
   <sheets>
     <sheet name="0 Comms" sheetId="11" r:id="rId1"/>
@@ -23,17 +23,6 @@
     <sheet name="Getting Involved" sheetId="6" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Worksheet!$M$42</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Worksheet!$M$43</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Worksheet!$N$46:$U$46</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Worksheet!$M$44</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Worksheet!$M$45</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Worksheet!$M$46</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Worksheet!$N$41:$U$41</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Worksheet!$N$42:$U$42</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Worksheet!$N$43:$U$43</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Worksheet!$N$44:$U$44</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Worksheet!$N$45:$U$45</definedName>
     <definedName name="AA">'2 Self-learning'!$XBR$21</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -47,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="321">
   <si>
     <t>Key stats</t>
   </si>
@@ -1168,6 +1157,75 @@
   </si>
   <si>
     <t>Aerial Duels win %</t>
+  </si>
+  <si>
+    <t>central mid</t>
+  </si>
+  <si>
+    <t>raw metric</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>Aggression</t>
+  </si>
+  <si>
+    <t>Competitiveness</t>
+  </si>
+  <si>
+    <t>Decisions(off the ball)</t>
+  </si>
+  <si>
+    <t>Positioning</t>
+  </si>
+  <si>
+    <t>Ball winner</t>
+  </si>
+  <si>
+    <t>new metric name</t>
+  </si>
+  <si>
+    <t>Fouls per 90 prank</t>
+  </si>
+  <si>
+    <t>Sliding tackles per 90 prank</t>
+  </si>
+  <si>
+    <t>Defensive duels per 90 prank</t>
+  </si>
+  <si>
+    <t>Yellow cards per 90 prank</t>
+  </si>
+  <si>
+    <t>Shots blocked per 90 prank</t>
+  </si>
+  <si>
+    <t>Received passes per 90 prank</t>
+  </si>
+  <si>
+    <t>Interceptions per 90 prank</t>
+  </si>
+  <si>
+    <t>weight add to 1 validation</t>
+  </si>
+  <si>
+    <t>Overall</t>
+  </si>
+  <si>
+    <t>Deep lying playmaker</t>
+  </si>
+  <si>
+    <t>Attacking playmaker</t>
+  </si>
+  <si>
+    <t>Runner</t>
+  </si>
+  <si>
+    <t>Tempo</t>
+  </si>
+  <si>
+    <t>position</t>
   </si>
 </sst>
 </file>
@@ -1424,7 +1482,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1560,14 +1618,8 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -1590,6 +1642,18 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -2533,6 +2597,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="762437999"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -4486,10 +4551,10 @@
       <c r="C12" s="32"/>
       <c r="D12" s="32"/>
       <c r="E12" s="32"/>
-      <c r="F12" s="69" t="s">
+      <c r="F12" s="87" t="s">
         <v>169</v>
       </c>
-      <c r="G12" s="69"/>
+      <c r="G12" s="87"/>
       <c r="N12" s="33"/>
       <c r="O12" s="33"/>
       <c r="P12" s="33"/>
@@ -4525,10 +4590,10 @@
       <c r="E14" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="F14" s="69" t="s">
+      <c r="F14" s="87" t="s">
         <v>73</v>
       </c>
-      <c r="G14" s="69"/>
+      <c r="G14" s="87"/>
       <c r="H14" s="33" t="s">
         <v>166</v>
       </c>
@@ -4550,10 +4615,10 @@
       <c r="E15" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="F15" s="69" t="s">
+      <c r="F15" s="87" t="s">
         <v>76</v>
       </c>
-      <c r="G15" s="69"/>
+      <c r="G15" s="87"/>
       <c r="H15" s="33" t="s">
         <v>165</v>
       </c>
@@ -5149,8 +5214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A82DF0DB-5968-4B43-A8AA-4F8D1A6A0F46}">
   <dimension ref="B2:V46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+    <sheetView zoomScale="87" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5163,7 +5228,7 @@
     <col min="9" max="9" width="8.6640625" customWidth="1"/>
     <col min="10" max="10" width="8.33203125" customWidth="1"/>
     <col min="11" max="11" width="11.33203125" customWidth="1"/>
-    <col min="13" max="13" width="14.1640625" customWidth="1"/>
+    <col min="13" max="13" width="7.33203125" customWidth="1"/>
     <col min="14" max="14" width="14.5" customWidth="1"/>
     <col min="15" max="15" width="14.5" bestFit="1" customWidth="1"/>
     <col min="16" max="18" width="14.5" customWidth="1"/>
@@ -5299,7 +5364,7 @@
       <c r="P9">
         <v>2.63</v>
       </c>
-      <c r="Q9" s="72">
+      <c r="Q9" s="70">
         <f>O9/P9-1</f>
         <v>4.5627376425855459E-2</v>
       </c>
@@ -5328,7 +5393,7 @@
       <c r="P10">
         <v>2.63</v>
       </c>
-      <c r="Q10" s="72">
+      <c r="Q10" s="70">
         <f>O10/P10-1</f>
         <v>3.8022813688214363E-3</v>
       </c>
@@ -5365,7 +5430,7 @@
       <c r="P12">
         <v>2.25</v>
       </c>
-      <c r="Q12" s="73">
+      <c r="Q12" s="71">
         <f>O12/P12-1</f>
         <v>0.17333333333333334</v>
       </c>
@@ -5386,8 +5451,8 @@
       <c r="P13">
         <v>2.25</v>
       </c>
-      <c r="Q13" s="73">
-        <f t="shared" ref="Q13:Q16" si="0">O13/P13-1</f>
+      <c r="Q13" s="71">
+        <f>O13/P13-1</f>
         <v>0.12444444444444436</v>
       </c>
     </row>
@@ -5406,8 +5471,8 @@
       <c r="P14">
         <v>2.25</v>
       </c>
-      <c r="Q14" s="73">
-        <f t="shared" si="0"/>
+      <c r="Q14" s="71">
+        <f>O14/P14-1</f>
         <v>9.3333333333333268E-2</v>
       </c>
     </row>
@@ -5426,8 +5491,8 @@
       <c r="P15">
         <v>2.25</v>
       </c>
-      <c r="Q15" s="73">
-        <f t="shared" si="0"/>
+      <c r="Q15" s="71">
+        <f>O15/P15-1</f>
         <v>4.888888888888876E-2</v>
       </c>
     </row>
@@ -5446,8 +5511,8 @@
       <c r="P16">
         <v>2.25</v>
       </c>
-      <c r="Q16" s="73">
-        <f t="shared" si="0"/>
+      <c r="Q16" s="71">
+        <f>O16/P16-1</f>
         <v>2.2222222222222143E-2</v>
       </c>
     </row>
@@ -5467,7 +5532,7 @@
       <c r="P18">
         <v>1.45</v>
       </c>
-      <c r="Q18" s="73">
+      <c r="Q18" s="71">
         <f>O18/P18-1</f>
         <v>0.64137931034482754</v>
       </c>
@@ -5488,8 +5553,8 @@
       <c r="P19">
         <v>1.45</v>
       </c>
-      <c r="Q19" s="73">
-        <f t="shared" ref="Q19:Q22" si="1">O19/P19-1</f>
+      <c r="Q19" s="71">
+        <f>O19/P19-1</f>
         <v>0.22758620689655173</v>
       </c>
     </row>
@@ -5506,8 +5571,8 @@
       <c r="P20">
         <v>1.45</v>
       </c>
-      <c r="Q20" s="73">
-        <f t="shared" si="1"/>
+      <c r="Q20" s="71">
+        <f>O20/P20-1</f>
         <v>0.1103448275862069</v>
       </c>
     </row>
@@ -5536,8 +5601,8 @@
       <c r="P21">
         <v>1.45</v>
       </c>
-      <c r="Q21" s="73">
-        <f t="shared" si="1"/>
+      <c r="Q21" s="71">
+        <f>O21/P21-1</f>
         <v>7.5862068965517393E-2</v>
       </c>
     </row>
@@ -5563,8 +5628,8 @@
       <c r="P22">
         <v>1.45</v>
       </c>
-      <c r="Q22" s="73">
-        <f t="shared" si="1"/>
+      <c r="Q22" s="71">
+        <f>O22/P22-1</f>
         <v>5.5172413793103559E-2</v>
       </c>
     </row>
@@ -5640,198 +5705,201 @@
       </c>
     </row>
     <row r="40" spans="3:22">
-      <c r="C40" s="74">
-        <f>5/7</f>
-        <v>0.7142857142857143</v>
-      </c>
-      <c r="D40" s="74">
+      <c r="C40" s="72">
+        <f>5/8</f>
+        <v>0.625</v>
+      </c>
+      <c r="D40" s="72">
         <f>3/13</f>
         <v>0.23076923076923078</v>
       </c>
     </row>
     <row r="41" spans="3:22">
-      <c r="C41" s="74">
-        <f>1/7</f>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="D41" s="74">
+      <c r="C41" s="72">
+        <f>1/8</f>
+        <v>0.125</v>
+      </c>
+      <c r="D41" s="72">
         <f>4/13</f>
         <v>0.30769230769230771</v>
       </c>
-      <c r="M41" s="79"/>
-      <c r="N41" s="80" t="s">
+      <c r="M41" s="77"/>
+      <c r="N41" s="78" t="s">
         <v>294</v>
       </c>
-      <c r="O41" s="80" t="s">
+      <c r="O41" s="78" t="s">
         <v>280</v>
       </c>
-      <c r="P41" s="80" t="s">
+      <c r="P41" s="78" t="s">
         <v>295</v>
       </c>
-      <c r="Q41" s="80" t="s">
+      <c r="Q41" s="78" t="s">
         <v>288</v>
       </c>
-      <c r="R41" s="80" t="s">
+      <c r="R41" s="78" t="s">
         <v>296</v>
       </c>
-      <c r="S41" s="80" t="s">
+      <c r="S41" s="78" t="s">
         <v>284</v>
       </c>
-      <c r="T41" s="80" t="s">
+      <c r="T41" s="78" t="s">
         <v>282</v>
       </c>
-      <c r="U41" s="81" t="s">
+      <c r="U41" s="79" t="s">
         <v>297</v>
       </c>
       <c r="V41" s="1"/>
     </row>
     <row r="42" spans="3:22">
-      <c r="C42" s="75"/>
-      <c r="D42" s="74">
+      <c r="C42" s="73">
+        <f>2/8</f>
+        <v>0.25</v>
+      </c>
+      <c r="D42" s="72">
         <f>6/13</f>
         <v>0.46153846153846156</v>
       </c>
-      <c r="M42" s="87" t="s">
+      <c r="M42" s="85" t="s">
         <v>261</v>
       </c>
-      <c r="N42" s="76">
+      <c r="N42" s="74">
         <v>0.12</v>
       </c>
-      <c r="O42" s="76">
+      <c r="O42" s="74">
         <v>0.23</v>
       </c>
-      <c r="P42" s="76">
+      <c r="P42" s="74">
         <v>0.18</v>
       </c>
-      <c r="Q42" s="77">
+      <c r="Q42" s="75">
         <v>6.03</v>
       </c>
-      <c r="R42" s="77">
+      <c r="R42" s="75">
         <v>0.15</v>
       </c>
-      <c r="S42" s="77">
+      <c r="S42" s="75">
         <v>31</v>
       </c>
-      <c r="T42" s="78">
+      <c r="T42" s="76">
         <v>1.62</v>
       </c>
-      <c r="U42" s="82">
+      <c r="U42" s="80">
         <v>71.400000000000006</v>
       </c>
     </row>
     <row r="43" spans="3:22">
-      <c r="M43" s="87" t="s">
+      <c r="M43" s="85" t="s">
         <v>290</v>
       </c>
-      <c r="N43" s="76">
+      <c r="N43" s="74">
         <v>0.24</v>
       </c>
-      <c r="O43" s="76">
+      <c r="O43" s="74">
         <v>0.14000000000000001</v>
       </c>
-      <c r="P43" s="76">
+      <c r="P43" s="74">
         <v>0.14000000000000001</v>
       </c>
-      <c r="Q43" s="77">
+      <c r="Q43" s="75">
         <v>4.25</v>
       </c>
-      <c r="R43" s="77">
+      <c r="R43" s="75">
         <v>0.39</v>
       </c>
-      <c r="S43" s="77">
+      <c r="S43" s="75">
         <v>28.5</v>
       </c>
-      <c r="T43" s="78">
+      <c r="T43" s="76">
         <v>0.39</v>
       </c>
-      <c r="U43" s="82">
+      <c r="U43" s="80">
         <v>45.1</v>
       </c>
     </row>
     <row r="44" spans="3:22">
-      <c r="M44" s="87" t="s">
+      <c r="M44" s="85" t="s">
         <v>291</v>
       </c>
-      <c r="N44" s="76">
+      <c r="N44" s="74">
         <v>0.06</v>
       </c>
-      <c r="O44" s="76">
+      <c r="O44" s="74">
         <v>0.06</v>
       </c>
-      <c r="P44" s="76">
+      <c r="P44" s="74">
         <v>0.11</v>
       </c>
-      <c r="Q44" s="77">
+      <c r="Q44" s="75">
         <v>3.17</v>
       </c>
-      <c r="R44" s="77">
+      <c r="R44" s="75">
         <v>0.14000000000000001</v>
       </c>
-      <c r="S44" s="77">
+      <c r="S44" s="75">
         <v>31.7</v>
       </c>
-      <c r="T44" s="78">
+      <c r="T44" s="76">
         <v>0.63</v>
       </c>
-      <c r="U44" s="82">
+      <c r="U44" s="80">
         <v>71.099999999999994</v>
       </c>
     </row>
     <row r="45" spans="3:22">
-      <c r="M45" s="87" t="s">
+      <c r="M45" s="85" t="s">
         <v>292</v>
       </c>
-      <c r="N45" s="76">
+      <c r="N45" s="74">
         <v>0.06</v>
       </c>
-      <c r="O45" s="76">
+      <c r="O45" s="74">
         <v>0.1</v>
       </c>
-      <c r="P45" s="76">
+      <c r="P45" s="74">
         <v>0.08</v>
       </c>
-      <c r="Q45" s="77">
+      <c r="Q45" s="75">
         <v>1.82</v>
       </c>
-      <c r="R45" s="77">
+      <c r="R45" s="75">
         <v>0.08</v>
       </c>
-      <c r="S45" s="77">
+      <c r="S45" s="75">
         <v>17.399999999999999</v>
       </c>
-      <c r="T45" s="78">
+      <c r="T45" s="76">
         <v>0.3</v>
       </c>
-      <c r="U45" s="82">
+      <c r="U45" s="80">
         <v>67.599999999999994</v>
       </c>
     </row>
     <row r="46" spans="3:22">
-      <c r="M46" s="88" t="s">
+      <c r="M46" s="86" t="s">
         <v>293</v>
       </c>
-      <c r="N46" s="83">
+      <c r="N46" s="81">
         <v>0.09</v>
       </c>
-      <c r="O46" s="83">
+      <c r="O46" s="81">
         <v>0.25</v>
       </c>
-      <c r="P46" s="83">
+      <c r="P46" s="81">
         <v>0.27</v>
       </c>
-      <c r="Q46" s="84">
+      <c r="Q46" s="82">
         <v>8.4700000000000006</v>
       </c>
-      <c r="R46" s="84">
+      <c r="R46" s="82">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="S46" s="84">
+      <c r="S46" s="82">
         <v>25.4</v>
       </c>
-      <c r="T46" s="85">
+      <c r="T46" s="83">
         <v>0.27</v>
       </c>
-      <c r="U46" s="86">
+      <c r="U46" s="84">
         <v>64.7</v>
       </c>
     </row>
@@ -6819,7 +6887,7 @@
       <c r="B9" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="70" t="s">
+      <c r="D9" s="88" t="s">
         <v>30</v>
       </c>
       <c r="I9" t="s">
@@ -6830,7 +6898,7 @@
       <c r="B10" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="70"/>
+      <c r="D10" s="88"/>
     </row>
     <row r="13" spans="1:9">
       <c r="B13" s="8" t="s">
@@ -6912,10 +6980,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6476FE99-38C7-4044-A99D-0C60D07A6712}">
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="I20" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="N36" sqref="N36:N40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6925,7 +6993,9 @@
     <col min="5" max="5" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11" customWidth="1"/>
+    <col min="10" max="10" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.1640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6962,11 +7032,11 @@
         <v>54</v>
       </c>
       <c r="H4" s="8"/>
-      <c r="I4" s="71" t="s">
+      <c r="I4" s="89" t="s">
         <v>32</v>
       </c>
-      <c r="J4" s="70"/>
-      <c r="K4" s="70"/>
+      <c r="J4" s="88"/>
+      <c r="K4" s="88"/>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="8"/>
@@ -6974,9 +7044,9 @@
         <v>150</v>
       </c>
       <c r="H5" s="8"/>
-      <c r="I5" s="70"/>
-      <c r="J5" s="70"/>
-      <c r="K5" s="70"/>
+      <c r="I5" s="88"/>
+      <c r="J5" s="88"/>
+      <c r="K5" s="88"/>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="8"/>
@@ -7077,12 +7147,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="2:8">
+    <row r="17" spans="2:14">
       <c r="B17" s="8" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="20" spans="2:8">
+    <row r="20" spans="2:14">
       <c r="B20" s="23" t="s">
         <v>203</v>
       </c>
@@ -7092,7 +7162,7 @@
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
     </row>
-    <row r="21" spans="2:8">
+    <row r="21" spans="2:14">
       <c r="C21" s="5" t="s">
         <v>79</v>
       </c>
@@ -7101,8 +7171,23 @@
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
-    </row>
-    <row r="22" spans="2:8">
+      <c r="J21" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="N21" s="4" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14">
       <c r="C22" s="18">
         <v>1</v>
       </c>
@@ -7121,8 +7206,24 @@
       <c r="H22" s="18" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="23" spans="2:8">
+      <c r="J22" s="17" t="s">
+        <v>298</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="L22" s="90" t="s">
+        <v>307</v>
+      </c>
+      <c r="M22" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="N22" s="88">
+        <f>SUM(M22:M25)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14">
       <c r="C23" s="17" t="s">
         <v>73</v>
       </c>
@@ -7141,8 +7242,21 @@
       <c r="H23" s="17">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="2:8">
+      <c r="J23" s="17" t="s">
+        <v>298</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="L23" s="90" t="s">
+        <v>308</v>
+      </c>
+      <c r="M23" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="N23" s="88"/>
+    </row>
+    <row r="24" spans="2:14">
       <c r="C24" s="17" t="s">
         <v>72</v>
       </c>
@@ -7159,8 +7273,21 @@
       <c r="H24" s="17">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="2:8">
+      <c r="J24" s="17" t="s">
+        <v>298</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="L24" s="90" t="s">
+        <v>309</v>
+      </c>
+      <c r="M24" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="N24" s="88"/>
+    </row>
+    <row r="25" spans="2:14">
       <c r="C25" s="17" t="s">
         <v>71</v>
       </c>
@@ -7177,8 +7304,21 @@
       <c r="H25" s="17">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="2:8">
+      <c r="J25" s="17" t="s">
+        <v>298</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="L25" s="90" t="s">
+        <v>310</v>
+      </c>
+      <c r="M25" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="N25" s="88"/>
+    </row>
+    <row r="26" spans="2:14">
       <c r="C26" s="19" t="s">
         <v>76</v>
       </c>
@@ -7195,8 +7335,24 @@
       <c r="H26" s="19">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="2:8">
+      <c r="J26" s="17" t="s">
+        <v>298</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="L26" s="90" t="s">
+        <v>309</v>
+      </c>
+      <c r="M26" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="N26" s="88">
+        <f>SUM(M26:M28)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14">
       <c r="C27" s="17"/>
       <c r="D27" s="17"/>
       <c r="E27" s="17" t="s">
@@ -7211,8 +7367,21 @@
       <c r="H27" s="17">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="2:8">
+      <c r="J27" s="17" t="s">
+        <v>298</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="L27" s="90" t="s">
+        <v>308</v>
+      </c>
+      <c r="M27" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="N27" s="88"/>
+    </row>
+    <row r="28" spans="2:14">
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
       <c r="E28" s="17" t="s">
@@ -7227,8 +7396,21 @@
       <c r="H28" s="17">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="2:8">
+      <c r="J28" s="17" t="s">
+        <v>298</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="L28" s="90" t="s">
+        <v>311</v>
+      </c>
+      <c r="M28" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="N28" s="88"/>
+    </row>
+    <row r="29" spans="2:14">
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
       <c r="E29" s="17" t="s">
@@ -7243,8 +7425,24 @@
       <c r="H29" s="17">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="2:8">
+      <c r="J29" s="17" t="s">
+        <v>298</v>
+      </c>
+      <c r="K29" s="17" t="s">
+        <v>303</v>
+      </c>
+      <c r="L29" s="90" t="s">
+        <v>312</v>
+      </c>
+      <c r="M29" s="3">
+        <v>1</v>
+      </c>
+      <c r="N29" s="69">
+        <f>M29</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14">
       <c r="C30" s="17" t="s">
         <v>92</v>
       </c>
@@ -7261,8 +7459,23 @@
       <c r="H30" s="17">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="2:8">
+      <c r="J30" s="17" t="s">
+        <v>298</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="L30" s="90" t="s">
+        <v>311</v>
+      </c>
+      <c r="M30" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="N30" s="88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14">
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="17" t="s">
@@ -7277,10 +7490,173 @@
       <c r="H31" s="17">
         <v>0</v>
       </c>
+      <c r="J31" s="17" t="s">
+        <v>298</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="L31" s="90" t="s">
+        <v>313</v>
+      </c>
+      <c r="M31" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="N31" s="88"/>
+    </row>
+    <row r="32" spans="2:14">
+      <c r="J32" s="17" t="s">
+        <v>298</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="L32" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="M32" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="N32" s="88">
+        <f>SUM(M32:M35)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="10:14">
+      <c r="J33" s="17" t="s">
+        <v>298</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="L33" s="90" t="s">
+        <v>302</v>
+      </c>
+      <c r="M33" s="3">
+        <v>0.35</v>
+      </c>
+      <c r="N33" s="88"/>
+    </row>
+    <row r="34" spans="10:14">
+      <c r="J34" s="17" t="s">
+        <v>298</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="L34" s="90" t="s">
+        <v>303</v>
+      </c>
+      <c r="M34" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="N34" s="88"/>
+    </row>
+    <row r="35" spans="10:14">
+      <c r="J35" s="17" t="s">
+        <v>298</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="L35" s="90" t="s">
+        <v>304</v>
+      </c>
+      <c r="M35" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="N35" s="88"/>
+    </row>
+    <row r="36" spans="10:14">
+      <c r="J36" s="17" t="s">
+        <v>298</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="L36" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="M36" s="3">
+        <f>0.2</f>
+        <v>0.2</v>
+      </c>
+      <c r="N36" s="88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="10:14">
+      <c r="J37" s="17" t="s">
+        <v>298</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="L37" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="M37" s="3">
+        <f t="shared" ref="M37:M40" si="0">0.2</f>
+        <v>0.2</v>
+      </c>
+      <c r="N37" s="88"/>
+    </row>
+    <row r="38" spans="10:14">
+      <c r="J38" s="17" t="s">
+        <v>298</v>
+      </c>
+      <c r="K38" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="L38" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="M38" s="3">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="N38" s="88"/>
+    </row>
+    <row r="39" spans="10:14">
+      <c r="J39" s="17" t="s">
+        <v>298</v>
+      </c>
+      <c r="K39" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="L39" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="M39" s="3">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="N39" s="88"/>
+    </row>
+    <row r="40" spans="10:14">
+      <c r="J40" s="17" t="s">
+        <v>298</v>
+      </c>
+      <c r="K40" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="L40" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="M40" s="3">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="N40" s="88"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="6">
+    <mergeCell ref="N36:N40"/>
     <mergeCell ref="I4:K5"/>
+    <mergeCell ref="N22:N25"/>
+    <mergeCell ref="N26:N28"/>
+    <mergeCell ref="N30:N31"/>
+    <mergeCell ref="N32:N35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>